<commit_message>
Inputs from text file called ListOfLinks. Only uses mode 2.
</commit_message>
<xml_diff>
--- a/Excel output/Crawl_9_10.xlsx
+++ b/Excel output/Crawl_9_10.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="646">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="647">
   <si>
     <t xml:space="preserve">
       About Google
@@ -462,7 +462,7 @@
     <t>Climatology</t>
   </si>
   <si>
-    <t>Climatology, Polar/Ice</t>
+    <t>Climatology, Forestry</t>
   </si>
   <si>
     <t>Commonwealth  Scientific and Industrial Research Organization (CSIRO) (Australia)</t>
@@ -492,9 +492,6 @@
     <t>Community, Image Collection, Web page</t>
   </si>
   <si>
-    <t>Consensus Effort, Data Service, Software</t>
-  </si>
-  <si>
     <t>Consultative  Group on International Agricultural Research</t>
   </si>
   <si>
@@ -1032,6 +1029,9 @@
     <t>MZ = Mozambique</t>
   </si>
   <si>
+    <t>Maps/Imaging, Spatial</t>
+  </si>
+  <si>
     <t>Montenegrin Academy  of Sciences and Arts</t>
   </si>
   <si>
@@ -1656,7 +1656,7 @@
     <t>['URL Type: http://cinergiterms.weebly.com/url-type.html', ['http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/bio.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/hydrobio.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/bio.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/hydrobio.jpg, '], ['http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/activity.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/activity.jpg, '], 'TLD: http://cinergiterms.weebly.com/top-level-domain.html', 'Country Code: http://cinergiterms.weebly.com/country-codes.html']</t>
   </si>
   <si>
-    <t>['URL Type: http://cinergiterms.weebly.com/url-type.html', ['http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/clima.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/clima.jpg, '], ['http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/software.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/software.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/software.jpg, '], 'TLD: http://cinergiterms.weebly.com/top-level-domain.html', 'Country Code: http://cinergiterms.weebly.com/country-codes.html']</t>
+    <t>['URL Type: http://cinergiterms.weebly.com/url-type.html', ['http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/clima.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/forestry.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/clima.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/forestry.jpg, '], ['http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/software.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/software.jpg, '], 'TLD: http://cinergiterms.weebly.com/top-level-domain.html', 'Country Code: http://cinergiterms.weebly.com/country-codes.html']</t>
   </si>
   <si>
     <t>['URL Type: http://cinergiterms.weebly.com/url-type.html', ['http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/clima.jpg, '], ['http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/software.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/software.jpg, '], 'TLD: http://cinergiterms.weebly.com/top-level-domain.html', 'Country Code: http://cinergiterms.weebly.com/country-codes.html']</t>
@@ -1671,6 +1671,9 @@
     <t>['URL Type: http://cinergiterms.weebly.com/url-type.html', ['http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/gis.jpg, '], ['http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/community.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/software.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/organization.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/community.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/software.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/organization.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/community.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/software.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/organization.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/community.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/software.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/organization.jpg, '], 'TLD: http://cinergiterms.weebly.com/top-level-domain.html', 'Country Code: http://cinergiterms.weebly.com/country-codes.html']</t>
   </si>
   <si>
+    <t>['URL Type: http://cinergiterms.weebly.com/url-type.html', ['http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/maps.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/spatial.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/maps.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/spatial.jpg, '], ['http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/community.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/software.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/community.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/software.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/community.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/software.jpg, '], 'TLD: http://cinergiterms.weebly.com/top-level-domain.html', 'Country Code: http://cinergiterms.weebly.com/country-codes.html']</t>
+  </si>
+  <si>
     <t>['URL Type: http://cinergiterms.weebly.com/url-type.html', ['http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/paleo.jpg, '], ['http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/community.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/community.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/community.jpg, '], 'TLD: http://cinergiterms.weebly.com/top-level-domain.html', 'Country Code: http://cinergiterms.weebly.com/country-codes.html']</t>
   </si>
   <si>
@@ -1692,9 +1695,6 @@
     <t>['URL Type: http://cinergiterms.weebly.com/url-type.html', [], ['http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/community.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/software.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/community.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/software.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/community.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/software.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/community.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/software.jpg, '], 'TLD: http://cinergiterms.weebly.com/top-level-domain.html', 'Country Code: http://cinergiterms.weebly.com/country-codes.html']</t>
   </si>
   <si>
-    <t>['URL Type: http://cinergiterms.weebly.com/url-type.html', [], ['http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/community.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/software.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/community.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/software.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/community.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/software.jpg, '], 'TLD: http://cinergiterms.weebly.com/top-level-domain.html', 'Country Code: http://cinergiterms.weebly.com/country-codes.html']</t>
-  </si>
-  <si>
     <t>['URL Type: http://cinergiterms.weebly.com/url-type.html', [], ['http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/community.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/software.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/forum.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/organization.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/community.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/software.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/forum.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/organization.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/community.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/software.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/forum.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/organization.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/community.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/software.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/forum.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/organization.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/community.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/software.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/forum.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/organization.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/community.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/software.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/forum.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/organization.jpg, '], 'TLD: http://cinergiterms.weebly.com/top-level-domain.html', 'Country Code: http://cinergiterms.weebly.com/country-codes.html']</t>
   </si>
   <si>
@@ -1833,6 +1833,9 @@
     <t>http://help.weebly.com/</t>
   </si>
   <si>
+    <t>http://howlattire.com</t>
+  </si>
+  <si>
     <t>http://inspiration.weebly.com/</t>
   </si>
   <si>
@@ -1860,9 +1863,6 @@
     <t>http://www.google.com/intl/en/options/</t>
   </si>
   <si>
-    <t>http://www.howlattire.com</t>
-  </si>
-  <si>
     <t>http://www.lifewatch.eu</t>
   </si>
   <si>
@@ -1876,6 +1876,9 @@
   </si>
   <si>
     <t>http://www.weebly.com/?utm_source=internal&amp;utm_medium=footer&amp;utm_campaign=3</t>
+  </si>
+  <si>
+    <t>http://www.weebly.com/?utm_source=internal&amp;utm_medium=footer&amp;utm_campaign=3#plans/compare</t>
   </si>
   <si>
     <t>http://www.weebly.com/?utm_source=internal&amp;utm_medium=footer&amp;utm_campaign=3#themes</t>
@@ -2308,9 +2311,9 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -2321,28 +2324,28 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
-      <c s="1" r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>489</v>
       </c>
-      <c s="1" r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>496</v>
       </c>
-      <c s="1" r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>377</v>
       </c>
-      <c s="1" r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>488</v>
       </c>
-      <c s="1" r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>409</v>
       </c>
-      <c s="1" r="F1" t="s">
-        <v>160</v>
-      </c>
-      <c s="1" r="G1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>457</v>
       </c>
-      <c s="1" r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>483</v>
       </c>
     </row>
@@ -2361,14 +2364,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" left="0.75" top="1" header="0.5" footer="0.5" right="0.75"/>
+  <pageMargins header="0.5" left="0.75" bottom="1" top="1" footer="0.5" right="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:H8"/>
   <sheetViews>
@@ -2379,28 +2382,28 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
-      <c s="1" r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>489</v>
       </c>
-      <c s="1" r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>496</v>
       </c>
-      <c s="1" r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>377</v>
       </c>
-      <c s="1" r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>488</v>
       </c>
-      <c s="1" r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>409</v>
       </c>
-      <c s="1" r="F1" t="s">
-        <v>160</v>
-      </c>
-      <c s="1" r="G1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>457</v>
       </c>
-      <c s="1" r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>483</v>
       </c>
     </row>
@@ -2426,13 +2429,13 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B3" t="s">
         <v>571</v>
       </c>
       <c r="C3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D3" t="s">
         <v>370</v>
@@ -2481,7 +2484,7 @@
         <v>135</v>
       </c>
       <c r="H5" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -2501,7 +2504,7 @@
         <v>372</v>
       </c>
       <c r="G6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H6" t="s">
         <v>561</v>
@@ -2509,13 +2512,13 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B7" t="s">
         <v>591</v>
       </c>
       <c r="C7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D7" t="s">
         <v>370</v>
@@ -2529,13 +2532,13 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B8" t="s">
         <v>614</v>
       </c>
       <c r="C8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D8" t="s">
         <v>370</v>
@@ -2548,16 +2551,16 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" left="0.75" top="1" header="0.5" footer="0.5" right="0.75"/>
+  <pageMargins header="0.5" left="0.75" bottom="1" top="1" footer="0.5" right="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H71"/>
+  <dimension ref="A1:H72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1" activeCell="A1"/>
@@ -2566,80 +2569,80 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
-      <c s="1" r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>489</v>
       </c>
-      <c s="1" r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>496</v>
       </c>
-      <c s="1" r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>377</v>
       </c>
-      <c s="1" r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>488</v>
       </c>
-      <c s="1" r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>409</v>
       </c>
-      <c s="1" r="F1" t="s">
-        <v>160</v>
-      </c>
-      <c s="1" r="G1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>457</v>
       </c>
-      <c s="1" r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>483</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>155</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C2" t="s">
-        <v>155</v>
+        <v>112</v>
       </c>
       <c r="D2" t="s">
         <v>370</v>
       </c>
       <c r="E2" t="s">
-        <v>372</v>
+        <v>463</v>
       </c>
       <c r="H2" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="C3" t="s">
-        <v>112</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
         <v>370</v>
       </c>
       <c r="E3" t="s">
-        <v>463</v>
+        <v>372</v>
       </c>
       <c r="H3" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>154</v>
       </c>
       <c r="B4" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>154</v>
       </c>
       <c r="D4" t="s">
         <v>370</v>
@@ -2668,38 +2671,38 @@
         <v>135</v>
       </c>
       <c r="H5" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>376</v>
       </c>
       <c r="B6" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>512</v>
       </c>
       <c r="D6" t="s">
-        <v>370</v>
+        <v>142</v>
       </c>
       <c r="E6" t="s">
-        <v>372</v>
+        <v>257</v>
       </c>
       <c r="H6" t="s">
-        <v>561</v>
+        <v>542</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>156</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C7" t="s">
-        <v>156</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
         <v>370</v>
@@ -2713,93 +2716,93 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>371</v>
+        <v>382</v>
       </c>
       <c r="B8" t="s">
-        <v>576</v>
+        <v>611</v>
       </c>
       <c r="C8" t="s">
-        <v>371</v>
+        <v>382</v>
       </c>
       <c r="D8" t="s">
-        <v>370</v>
+        <v>201</v>
       </c>
       <c r="E8" t="s">
-        <v>372</v>
+        <v>135</v>
       </c>
       <c r="H8" t="s">
-        <v>561</v>
+        <v>544</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>376</v>
+        <v>155</v>
       </c>
       <c r="B9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C9" t="s">
-        <v>512</v>
+        <v>155</v>
       </c>
       <c r="D9" t="s">
-        <v>142</v>
+        <v>370</v>
       </c>
       <c r="E9" t="s">
-        <v>258</v>
+        <v>372</v>
       </c>
       <c r="H9" t="s">
-        <v>542</v>
+        <v>561</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>382</v>
+        <v>486</v>
       </c>
       <c r="B10" t="s">
-        <v>611</v>
+        <v>567</v>
       </c>
       <c r="C10" t="s">
-        <v>382</v>
+        <v>486</v>
       </c>
       <c r="D10" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="E10" t="s">
-        <v>135</v>
+        <v>372</v>
       </c>
       <c r="H10" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>486</v>
+        <v>371</v>
       </c>
       <c r="B11" t="s">
-        <v>567</v>
+        <v>576</v>
       </c>
       <c r="C11" t="s">
-        <v>486</v>
+        <v>371</v>
       </c>
       <c r="D11" t="s">
-        <v>183</v>
+        <v>370</v>
       </c>
       <c r="E11" t="s">
         <v>372</v>
       </c>
       <c r="H11" t="s">
-        <v>543</v>
+        <v>561</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B12" t="s">
         <v>590</v>
       </c>
       <c r="C12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D12" t="s">
         <v>370</v>
@@ -2813,13 +2816,13 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>524</v>
+        <v>171</v>
       </c>
       <c r="B13" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="C13" t="s">
-        <v>524</v>
+        <v>171</v>
       </c>
       <c r="D13" t="s">
         <v>370</v>
@@ -2828,7 +2831,7 @@
         <v>372</v>
       </c>
       <c r="G13" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H13" t="s">
         <v>561</v>
@@ -2836,13 +2839,13 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>172</v>
+        <v>234</v>
       </c>
       <c r="B14" t="s">
-        <v>586</v>
+        <v>608</v>
       </c>
       <c r="C14" t="s">
-        <v>172</v>
+        <v>234</v>
       </c>
       <c r="D14" t="s">
         <v>370</v>
@@ -2850,131 +2853,131 @@
       <c r="E14" t="s">
         <v>372</v>
       </c>
-      <c r="G14" t="s">
-        <v>200</v>
-      </c>
       <c r="H14" t="s">
         <v>561</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>200</v>
+        <v>524</v>
       </c>
       <c r="B15" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="C15" t="s">
-        <v>200</v>
+        <v>524</v>
       </c>
       <c r="D15" t="s">
         <v>370</v>
       </c>
       <c r="E15" t="s">
-        <v>147</v>
+        <v>372</v>
       </c>
       <c r="G15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H15" t="s">
-        <v>552</v>
+        <v>561</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>235</v>
+        <v>199</v>
       </c>
       <c r="B16" t="s">
-        <v>607</v>
+        <v>588</v>
       </c>
       <c r="C16" t="s">
-        <v>235</v>
+        <v>199</v>
       </c>
       <c r="D16" t="s">
         <v>370</v>
       </c>
       <c r="E16" t="s">
-        <v>372</v>
+        <v>147</v>
+      </c>
+      <c r="G16" t="s">
+        <v>199</v>
       </c>
       <c r="H16" t="s">
-        <v>561</v>
+        <v>553</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>245</v>
+        <v>158</v>
       </c>
       <c r="B17" t="s">
-        <v>610</v>
+        <v>587</v>
       </c>
       <c r="C17" t="s">
-        <v>245</v>
+        <v>158</v>
       </c>
       <c r="D17" t="s">
-        <v>101</v>
+        <v>370</v>
       </c>
       <c r="E17" t="s">
-        <v>46</v>
+        <v>463</v>
+      </c>
+      <c r="G17" t="s">
+        <v>199</v>
       </c>
       <c r="H17" t="s">
-        <v>540</v>
+        <v>558</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>200</v>
+        <v>244</v>
       </c>
       <c r="B18" t="s">
-        <v>589</v>
+        <v>610</v>
       </c>
       <c r="C18" t="s">
-        <v>200</v>
+        <v>244</v>
       </c>
       <c r="D18" t="s">
-        <v>370</v>
+        <v>101</v>
       </c>
       <c r="E18" t="s">
-        <v>372</v>
-      </c>
-      <c r="G18" t="s">
-        <v>200</v>
+        <v>46</v>
       </c>
       <c r="H18" t="s">
-        <v>561</v>
+        <v>540</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>159</v>
+        <v>199</v>
       </c>
       <c r="B19" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="C19" t="s">
-        <v>159</v>
+        <v>199</v>
       </c>
       <c r="D19" t="s">
         <v>370</v>
       </c>
       <c r="E19" t="s">
-        <v>463</v>
+        <v>372</v>
       </c>
       <c r="G19" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H19" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B20" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="C20" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D20" t="s">
         <v>370</v>
@@ -2988,82 +2991,82 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B21" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="C21" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D21" t="s">
-        <v>370</v>
+        <v>464</v>
       </c>
       <c r="E21" t="s">
-        <v>152</v>
+        <v>372</v>
       </c>
       <c r="H21" t="s">
-        <v>556</v>
+        <v>548</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>401</v>
+        <v>232</v>
       </c>
       <c r="B22" t="s">
-        <v>597</v>
+        <v>609</v>
       </c>
       <c r="C22" t="s">
-        <v>401</v>
+        <v>232</v>
       </c>
       <c r="D22" t="s">
         <v>370</v>
       </c>
       <c r="E22" t="s">
-        <v>259</v>
+        <v>152</v>
       </c>
       <c r="H22" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>236</v>
+        <v>451</v>
       </c>
       <c r="B23" t="s">
-        <v>602</v>
+        <v>640</v>
       </c>
       <c r="C23" t="s">
-        <v>236</v>
+        <v>451</v>
       </c>
       <c r="D23" t="s">
-        <v>464</v>
+        <v>370</v>
       </c>
       <c r="E23" t="s">
         <v>372</v>
       </c>
       <c r="H23" t="s">
-        <v>547</v>
+        <v>561</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>451</v>
+        <v>401</v>
       </c>
       <c r="B24" t="s">
-        <v>639</v>
+        <v>597</v>
       </c>
       <c r="C24" t="s">
-        <v>451</v>
+        <v>401</v>
       </c>
       <c r="D24" t="s">
         <v>370</v>
       </c>
       <c r="E24" t="s">
-        <v>372</v>
+        <v>258</v>
       </c>
       <c r="H24" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -3108,36 +3111,36 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>1</v>
+        <v>402</v>
       </c>
       <c r="B27" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="C27" t="s">
-        <v>1</v>
+        <v>402</v>
       </c>
       <c r="D27" t="s">
-        <v>396</v>
+        <v>370</v>
       </c>
       <c r="E27" t="s">
-        <v>148</v>
+        <v>169</v>
       </c>
       <c r="H27" t="s">
-        <v>546</v>
+        <v>561</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>234</v>
+        <v>0</v>
       </c>
       <c r="B28" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="C28" t="s">
-        <v>234</v>
+        <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>399</v>
+        <v>370</v>
       </c>
       <c r="E28" t="s">
         <v>372</v>
@@ -3148,16 +3151,16 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>0</v>
+        <v>233</v>
       </c>
       <c r="B29" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C29" t="s">
-        <v>0</v>
+        <v>233</v>
       </c>
       <c r="D29" t="s">
-        <v>370</v>
+        <v>399</v>
       </c>
       <c r="E29" t="s">
         <v>372</v>
@@ -3168,62 +3171,62 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>402</v>
+        <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="C30" t="s">
-        <v>402</v>
+        <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>370</v>
+        <v>396</v>
       </c>
       <c r="E30" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
       <c r="H30" t="s">
-        <v>561</v>
+        <v>547</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>518</v>
+        <v>202</v>
       </c>
       <c r="B31" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="C31" t="s">
-        <v>518</v>
+        <v>202</v>
       </c>
       <c r="D31" t="s">
         <v>370</v>
       </c>
       <c r="E31" t="s">
-        <v>372</v>
+        <v>145</v>
       </c>
       <c r="H31" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>203</v>
+        <v>518</v>
       </c>
       <c r="B32" t="s">
-        <v>613</v>
+        <v>617</v>
       </c>
       <c r="C32" t="s">
-        <v>203</v>
+        <v>518</v>
       </c>
       <c r="D32" t="s">
         <v>370</v>
       </c>
       <c r="E32" t="s">
-        <v>145</v>
+        <v>372</v>
       </c>
       <c r="H32" t="s">
-        <v>557</v>
+        <v>561</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -3237,7 +3240,7 @@
         <v>519</v>
       </c>
       <c r="D33" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E33" t="s">
         <v>150</v>
@@ -3251,62 +3254,62 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>158</v>
+        <v>522</v>
       </c>
       <c r="B34" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="C34" t="s">
-        <v>158</v>
+        <v>522</v>
       </c>
       <c r="D34" t="s">
         <v>370</v>
       </c>
       <c r="E34" t="s">
-        <v>372</v>
+        <v>136</v>
       </c>
       <c r="H34" t="s">
-        <v>561</v>
+        <v>550</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>522</v>
+        <v>157</v>
       </c>
       <c r="B35" t="s">
         <v>618</v>
       </c>
       <c r="C35" t="s">
-        <v>522</v>
+        <v>157</v>
       </c>
       <c r="D35" t="s">
         <v>370</v>
       </c>
       <c r="E35" t="s">
-        <v>136</v>
+        <v>372</v>
       </c>
       <c r="H35" t="s">
-        <v>549</v>
+        <v>561</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" t="s">
-        <v>518</v>
+        <v>236</v>
       </c>
       <c r="B36" t="s">
-        <v>621</v>
+        <v>604</v>
       </c>
       <c r="C36" t="s">
-        <v>518</v>
+        <v>236</v>
       </c>
       <c r="D36" t="s">
-        <v>370</v>
+        <v>143</v>
       </c>
       <c r="E36" t="s">
-        <v>372</v>
+        <v>257</v>
       </c>
       <c r="H36" t="s">
-        <v>561</v>
+        <v>541</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -3323,50 +3326,50 @@
         <v>370</v>
       </c>
       <c r="E37" t="s">
-        <v>139</v>
+        <v>372</v>
       </c>
       <c r="H37" t="s">
-        <v>550</v>
+        <v>561</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>237</v>
+        <v>518</v>
       </c>
       <c r="B38" t="s">
-        <v>603</v>
+        <v>623</v>
       </c>
       <c r="C38" t="s">
-        <v>237</v>
+        <v>518</v>
       </c>
       <c r="D38" t="s">
-        <v>143</v>
+        <v>370</v>
       </c>
       <c r="E38" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="H38" t="s">
-        <v>541</v>
+        <v>551</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" t="s">
-        <v>520</v>
+        <v>260</v>
       </c>
       <c r="B39" t="s">
-        <v>582</v>
+        <v>601</v>
       </c>
       <c r="C39" t="s">
-        <v>520</v>
+        <v>260</v>
       </c>
       <c r="D39" t="s">
         <v>370</v>
       </c>
       <c r="E39" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H39" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -3391,39 +3394,39 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41" t="s">
-        <v>261</v>
+        <v>520</v>
       </c>
       <c r="B41" t="s">
-        <v>600</v>
+        <v>582</v>
       </c>
       <c r="C41" t="s">
-        <v>261</v>
+        <v>520</v>
       </c>
       <c r="D41" t="s">
         <v>370</v>
       </c>
       <c r="E41" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H41" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" t="s">
-        <v>186</v>
+        <v>518</v>
       </c>
       <c r="B42" t="s">
-        <v>604</v>
+        <v>583</v>
       </c>
       <c r="C42" t="s">
-        <v>186</v>
+        <v>518</v>
       </c>
       <c r="D42" t="s">
         <v>370</v>
       </c>
       <c r="E42" t="s">
-        <v>170</v>
+        <v>256</v>
       </c>
       <c r="H42" t="s">
         <v>561</v>
@@ -3431,19 +3434,19 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" t="s">
-        <v>518</v>
+        <v>185</v>
       </c>
       <c r="B43" t="s">
-        <v>583</v>
+        <v>605</v>
       </c>
       <c r="C43" t="s">
-        <v>518</v>
+        <v>185</v>
       </c>
       <c r="D43" t="s">
         <v>370</v>
       </c>
       <c r="E43" t="s">
-        <v>257</v>
+        <v>169</v>
       </c>
       <c r="H43" t="s">
         <v>561</v>
@@ -3474,7 +3477,7 @@
         <v>484</v>
       </c>
       <c r="B45" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="C45" t="s">
         <v>484</v>
@@ -3483,7 +3486,7 @@
         <v>370</v>
       </c>
       <c r="E45" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H45" t="s">
         <v>559</v>
@@ -3494,7 +3497,7 @@
         <v>403</v>
       </c>
       <c r="B46" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="C46" t="s">
         <v>403</v>
@@ -3514,7 +3517,7 @@
         <v>4</v>
       </c>
       <c r="B47" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="C47" t="s">
         <v>4</v>
@@ -3526,7 +3529,7 @@
         <v>372</v>
       </c>
       <c r="G47" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H47" t="s">
         <v>561</v>
@@ -3537,22 +3540,22 @@
         <v>523</v>
       </c>
       <c r="B48" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C48" t="s">
         <v>523</v>
       </c>
       <c r="D48" t="s">
-        <v>370</v>
+        <v>332</v>
       </c>
       <c r="E48" t="s">
         <v>151</v>
       </c>
       <c r="G48" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H48" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -3560,7 +3563,7 @@
         <v>452</v>
       </c>
       <c r="B49" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="C49" t="s">
         <v>452</v>
@@ -3580,7 +3583,7 @@
         <v>453</v>
       </c>
       <c r="B50" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="C50" t="s">
         <v>453</v>
@@ -3600,7 +3603,7 @@
         <v>533</v>
       </c>
       <c r="B51" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="C51" t="s">
         <v>533</v>
@@ -3620,7 +3623,7 @@
         <v>454</v>
       </c>
       <c r="B52" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="C52" t="s">
         <v>454</v>
@@ -3637,19 +3640,19 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B53" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="C53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D53" t="s">
         <v>370</v>
       </c>
       <c r="E53" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H53" t="s">
         <v>561</v>
@@ -3660,7 +3663,7 @@
         <v>515</v>
       </c>
       <c r="B54" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="C54" t="s">
         <v>515</v>
@@ -3677,13 +3680,13 @@
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B55" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="C55" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D55" t="s">
         <v>370</v>
@@ -3697,13 +3700,13 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="B56" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="C56" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="D56" t="s">
         <v>370</v>
@@ -3717,13 +3720,13 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="B57" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="C57" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="D57" t="s">
         <v>370</v>
@@ -3737,13 +3740,13 @@
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="B58" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="C58" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="D58" t="s">
         <v>370</v>
@@ -3757,13 +3760,13 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>246</v>
+        <v>5</v>
       </c>
       <c r="B59" t="s">
-        <v>609</v>
+        <v>638</v>
       </c>
       <c r="C59" t="s">
-        <v>246</v>
+        <v>5</v>
       </c>
       <c r="D59" t="s">
         <v>370</v>
@@ -3777,13 +3780,13 @@
     </row>
     <row r="60" spans="1:8">
       <c r="A60" t="s">
-        <v>5</v>
+        <v>245</v>
       </c>
       <c r="B60" t="s">
-        <v>637</v>
+        <v>600</v>
       </c>
       <c r="C60" t="s">
-        <v>5</v>
+        <v>245</v>
       </c>
       <c r="D60" t="s">
         <v>370</v>
@@ -3797,13 +3800,13 @@
     </row>
     <row r="61" spans="1:8">
       <c r="A61" t="s">
-        <v>501</v>
+        <v>644</v>
       </c>
       <c r="B61" t="s">
-        <v>565</v>
+        <v>633</v>
       </c>
       <c r="C61" t="s">
-        <v>501</v>
+        <v>644</v>
       </c>
       <c r="D61" t="s">
         <v>370</v>
@@ -3817,13 +3820,13 @@
     </row>
     <row r="62" spans="1:8">
       <c r="A62" t="s">
-        <v>643</v>
+        <v>168</v>
       </c>
       <c r="B62" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C62" t="s">
-        <v>643</v>
+        <v>168</v>
       </c>
       <c r="D62" t="s">
         <v>370</v>
@@ -3837,13 +3840,13 @@
     </row>
     <row r="63" spans="1:8">
       <c r="A63" t="s">
-        <v>169</v>
+        <v>501</v>
       </c>
       <c r="B63" t="s">
-        <v>630</v>
+        <v>565</v>
       </c>
       <c r="C63" t="s">
-        <v>169</v>
+        <v>501</v>
       </c>
       <c r="D63" t="s">
         <v>370</v>
@@ -3857,19 +3860,19 @@
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="B64" t="s">
         <v>563</v>
       </c>
       <c r="C64" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="D64" t="s">
         <v>370</v>
       </c>
       <c r="E64" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H64" t="s">
         <v>561</v>
@@ -3917,116 +3920,136 @@
     </row>
     <row r="67" spans="1:8">
       <c r="A67" t="s">
-        <v>203</v>
+        <v>517</v>
       </c>
       <c r="B67" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="C67" t="s">
-        <v>203</v>
+        <v>517</v>
       </c>
       <c r="D67" t="s">
-        <v>370</v>
+        <v>72</v>
       </c>
       <c r="E67" t="s">
-        <v>145</v>
+        <v>463</v>
+      </c>
+      <c r="G67" t="s">
+        <v>491</v>
       </c>
       <c r="H67" t="s">
-        <v>557</v>
+        <v>539</v>
       </c>
     </row>
     <row r="68" spans="1:8">
       <c r="A68" t="s">
-        <v>522</v>
+        <v>202</v>
       </c>
       <c r="B68" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="C68" t="s">
-        <v>522</v>
+        <v>202</v>
       </c>
       <c r="D68" t="s">
         <v>370</v>
       </c>
       <c r="E68" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="H68" t="s">
-        <v>549</v>
+        <v>557</v>
       </c>
     </row>
     <row r="69" spans="1:8">
       <c r="A69" t="s">
-        <v>522</v>
+        <v>202</v>
       </c>
       <c r="B69" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="C69" t="s">
-        <v>522</v>
+        <v>202</v>
       </c>
       <c r="D69" t="s">
         <v>370</v>
       </c>
       <c r="E69" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="H69" t="s">
-        <v>549</v>
+        <v>557</v>
       </c>
     </row>
     <row r="70" spans="1:8">
       <c r="A70" t="s">
-        <v>517</v>
+        <v>533</v>
       </c>
       <c r="B70" t="s">
-        <v>612</v>
+        <v>637</v>
       </c>
       <c r="C70" t="s">
-        <v>517</v>
+        <v>533</v>
       </c>
       <c r="D70" t="s">
-        <v>72</v>
+        <v>370</v>
       </c>
       <c r="E70" t="s">
-        <v>463</v>
-      </c>
-      <c r="G70" t="s">
-        <v>491</v>
+        <v>372</v>
       </c>
       <c r="H70" t="s">
-        <v>539</v>
+        <v>561</v>
       </c>
     </row>
     <row r="71" spans="1:8">
       <c r="A71" t="s">
-        <v>533</v>
+        <v>522</v>
       </c>
       <c r="B71" t="s">
-        <v>636</v>
+        <v>621</v>
       </c>
       <c r="C71" t="s">
-        <v>533</v>
+        <v>522</v>
       </c>
       <c r="D71" t="s">
         <v>370</v>
       </c>
       <c r="E71" t="s">
-        <v>372</v>
+        <v>136</v>
       </c>
       <c r="H71" t="s">
-        <v>561</v>
+        <v>550</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72" t="s">
+        <v>522</v>
+      </c>
+      <c r="B72" t="s">
+        <v>620</v>
+      </c>
+      <c r="C72" t="s">
+        <v>522</v>
+      </c>
+      <c r="D72" t="s">
+        <v>370</v>
+      </c>
+      <c r="E72" t="s">
+        <v>136</v>
+      </c>
+      <c r="H72" t="s">
+        <v>550</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" left="0.75" top="1" header="0.5" footer="0.5" right="0.75"/>
+  <pageMargins header="0.5" left="0.75" bottom="1" top="1" footer="0.5" right="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
@@ -4036,14 +4059,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins bottom="1" left="0.75" top="1" header="0.5" footer="0.5" right="0.75"/>
+  <pageMargins header="0.5" left="0.75" bottom="1" top="1" footer="0.5" right="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:A183"/>
   <sheetViews>
@@ -4390,222 +4413,222 @@
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="113" spans="1:1">
@@ -4964,14 +4987,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" left="0.75" top="1" header="0.5" footer="0.5" right="0.75"/>
+  <pageMargins header="0.5" left="0.75" bottom="1" top="1" footer="0.5" right="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:A253"/>
   <sheetViews>
@@ -5248,497 +5271,497 @@
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="153" spans="1:1">
@@ -6203,22 +6226,22 @@
     </row>
     <row r="245" spans="1:1">
       <c r="A245" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="246" spans="1:1">
       <c r="A246" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="247" spans="1:1">
       <c r="A247" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="248" spans="1:1">
       <c r="A248" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="249" spans="1:1">
@@ -6243,10 +6266,10 @@
     </row>
     <row r="253" spans="1:1">
       <c r="A253" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" left="0.75" top="1" header="0.5" footer="0.5" right="0.75"/>
+  <pageMargins header="0.5" left="0.75" bottom="1" top="1" footer="0.5" right="0.75"/>
 </worksheet>
 </file>
</xml_diff>